<commit_message>
Updates for slides for Will
</commit_message>
<xml_diff>
--- a/11-Parameters/carbon-2.xlsx
+++ b/11-Parameters/carbon-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2062944630955/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{099C0C49-7461-7845-90DF-8FE791F5E1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{099C0C49-7461-7845-90DF-8FE791F5E1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DA75AA5-A8C0-0F4E-AC45-DFEA849EAD3A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LhARABeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,8 +888,8 @@
         <v>71</v>
       </c>
       <c r="F3" s="10">
-        <f>45.6095</f>
-        <v>45.609499999999997</v>
+        <f>45.60947984</f>
+        <v>45.609479839999999</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>11</v>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="F9" s="11">
         <f>F3</f>
-        <v>45.609499999999997</v>
+        <v>45.609479839999999</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>11</v>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="F10" s="11">
         <f>0.02*F9</f>
-        <v>0.91218999999999995</v>
+        <v>0.9121895968</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>11</v>

</xml_diff>